<commit_message>
Added Excel file permission error handling method.
</commit_message>
<xml_diff>
--- a/updated_test_table.xlsx
+++ b/updated_test_table.xlsx
@@ -495,10 +495,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F2" t="n">
+        <v>21</v>
       </c>
       <c r="G2" t="inlineStr"/>
     </row>
@@ -526,10 +524,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F3" t="n">
+        <v>48</v>
       </c>
       <c r="G3" t="inlineStr"/>
     </row>
@@ -557,10 +553,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F4" t="n">
+        <v>35</v>
       </c>
       <c r="G4" t="inlineStr"/>
     </row>
@@ -588,10 +582,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F5" t="n">
+        <v>45</v>
       </c>
       <c r="G5" t="inlineStr"/>
     </row>
@@ -619,10 +611,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F6" t="n">
+        <v>56</v>
       </c>
       <c r="G6" t="inlineStr"/>
     </row>
@@ -650,10 +640,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F7" t="n">
+        <v>58</v>
       </c>
       <c r="G7" t="inlineStr"/>
     </row>
@@ -681,10 +669,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F8" t="n">
+        <v>59</v>
       </c>
       <c r="G8" t="inlineStr"/>
     </row>
@@ -712,10 +698,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F9" t="n">
+        <v>57</v>
       </c>
       <c r="G9" t="inlineStr"/>
     </row>
@@ -778,10 +762,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F11" t="n">
+        <v>33</v>
       </c>
       <c r="G11" t="inlineStr"/>
     </row>
@@ -809,10 +791,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F12" t="n">
+        <v>76</v>
       </c>
       <c r="G12" t="inlineStr"/>
     </row>
@@ -840,10 +820,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F13" t="n">
+        <v>41</v>
       </c>
       <c r="G13" t="inlineStr"/>
     </row>
@@ -871,10 +849,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F14" t="n">
+        <v>61</v>
       </c>
       <c r="G14" t="inlineStr"/>
     </row>
@@ -902,10 +878,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F15" t="n">
+        <v>49</v>
       </c>
       <c r="G15" t="inlineStr"/>
     </row>
@@ -968,10 +942,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F17" t="n">
+        <v>64</v>
       </c>
       <c r="G17" t="inlineStr"/>
     </row>
@@ -999,10 +971,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F18" t="n">
+        <v>63</v>
       </c>
       <c r="G18" t="inlineStr"/>
     </row>
@@ -1030,10 +1000,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F19" t="n">
+        <v>47</v>
       </c>
       <c r="G19" t="inlineStr"/>
     </row>
@@ -1061,10 +1029,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F20" t="n">
+        <v>68</v>
       </c>
       <c r="G20" t="inlineStr"/>
     </row>
@@ -1092,10 +1058,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F21" t="n">
+        <v>75</v>
       </c>
       <c r="G21" t="inlineStr"/>
     </row>
@@ -1123,10 +1087,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F22" t="n">
+        <v>52</v>
       </c>
       <c r="G22" t="inlineStr"/>
     </row>
@@ -1154,10 +1116,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F23" t="n">
+        <v>57</v>
       </c>
       <c r="G23" t="inlineStr"/>
     </row>
@@ -1185,10 +1145,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F24" t="n">
+        <v>56</v>
       </c>
       <c r="G24" t="inlineStr"/>
     </row>
@@ -1216,10 +1174,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F25" t="n">
+        <v>73</v>
       </c>
       <c r="G25" t="inlineStr"/>
     </row>
@@ -1247,10 +1203,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F26" t="n">
+        <v>67</v>
       </c>
       <c r="G26" t="inlineStr"/>
     </row>
@@ -1278,10 +1232,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F27" t="n">
+        <v>61</v>
       </c>
       <c r="G27" t="inlineStr"/>
     </row>
@@ -1309,10 +1261,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F28" t="n">
+        <v>92</v>
       </c>
       <c r="G28" t="inlineStr"/>
     </row>
@@ -1340,10 +1290,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F29" t="n">
+        <v>71</v>
       </c>
       <c r="G29" t="inlineStr"/>
     </row>
@@ -1371,10 +1319,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F30" t="n">
+        <v>95</v>
       </c>
       <c r="G30" t="inlineStr"/>
     </row>
@@ -1402,10 +1348,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F31" t="n">
+        <v>40</v>
       </c>
       <c r="G31" t="inlineStr"/>
     </row>
@@ -1433,10 +1377,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F32" t="n">
+        <v>30</v>
       </c>
       <c r="G32" t="inlineStr"/>
     </row>
@@ -1464,10 +1406,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F33" t="n">
+        <v>41</v>
       </c>
       <c r="G33" t="inlineStr"/>
     </row>
@@ -1495,10 +1435,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F34" t="n">
+        <v>46</v>
       </c>
       <c r="G34" t="inlineStr"/>
     </row>
@@ -1526,10 +1464,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F35" t="n">
+        <v>33</v>
       </c>
       <c r="G35" t="inlineStr"/>
     </row>
@@ -1557,10 +1493,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F36" t="n">
+        <v>47</v>
       </c>
       <c r="G36" t="inlineStr"/>
     </row>
@@ -1588,10 +1522,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F37" t="n">
+        <v>40</v>
       </c>
       <c r="G37" t="inlineStr"/>
     </row>
@@ -1619,10 +1551,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F38" t="n">
+        <v>45</v>
       </c>
       <c r="G38" t="inlineStr"/>
     </row>
@@ -1650,10 +1580,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F39" t="n">
+        <v>88</v>
       </c>
       <c r="G39" t="inlineStr"/>
     </row>
@@ -1710,10 +1638,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F41" t="n">
+        <v>27</v>
       </c>
       <c r="G41" t="inlineStr"/>
     </row>
@@ -1770,10 +1696,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F43" t="n">
+        <v>54</v>
       </c>
       <c r="G43" t="inlineStr"/>
     </row>
@@ -1801,10 +1725,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F44" t="n">
+        <v>65</v>
       </c>
       <c r="G44" t="inlineStr"/>
     </row>
@@ -1832,10 +1754,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F45" t="n">
+        <v>54</v>
       </c>
       <c r="G45" t="inlineStr"/>
     </row>
@@ -1863,10 +1783,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F46" t="n">
+        <v>27</v>
       </c>
       <c r="G46" t="inlineStr"/>
     </row>
@@ -1894,10 +1812,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F47" t="n">
+        <v>28</v>
       </c>
       <c r="G47" t="inlineStr"/>
     </row>
@@ -1925,10 +1841,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F48" t="n">
+        <v>41</v>
       </c>
       <c r="G48" t="inlineStr"/>
     </row>
@@ -1956,10 +1870,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F49" t="n">
+        <v>48</v>
       </c>
       <c r="G49" t="inlineStr"/>
     </row>
@@ -2016,10 +1928,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F51" t="n">
+        <v>73</v>
       </c>
       <c r="G51" t="inlineStr"/>
     </row>
@@ -2076,10 +1986,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F53" t="n">
+        <v>50</v>
       </c>
       <c r="G53" t="inlineStr"/>
     </row>
@@ -2142,10 +2050,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F55" t="n">
+        <v>70</v>
       </c>
       <c r="G55" t="inlineStr"/>
     </row>
@@ -2173,10 +2079,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F56" t="n">
+        <v>58</v>
       </c>
       <c r="G56" t="inlineStr"/>
     </row>
@@ -2204,10 +2108,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F57" t="n">
+        <v>68</v>
       </c>
       <c r="G57" t="inlineStr"/>
     </row>
@@ -2235,10 +2137,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F58" t="n">
+        <v>62</v>
       </c>
       <c r="G58" t="inlineStr"/>
     </row>
@@ -2266,10 +2166,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F59" t="n">
+        <v>58</v>
       </c>
       <c r="G59" t="inlineStr"/>
     </row>
@@ -2326,10 +2224,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F61" t="n">
+        <v>45</v>
       </c>
       <c r="G61" t="inlineStr"/>
     </row>
@@ -2357,10 +2253,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F62" t="n">
+        <v>48</v>
       </c>
       <c r="G62" t="inlineStr"/>
     </row>
@@ -2388,10 +2282,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F63" t="n">
+        <v>75</v>
       </c>
       <c r="G63" t="inlineStr"/>
     </row>
@@ -2448,10 +2340,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F65" t="n">
+        <v>45</v>
       </c>
       <c r="G65" t="inlineStr"/>
     </row>
@@ -2508,10 +2398,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F67" t="n">
+        <v>46</v>
       </c>
       <c r="G67" t="inlineStr"/>
     </row>
@@ -2539,10 +2427,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F68" t="n">
+        <v>58</v>
       </c>
       <c r="G68" t="inlineStr"/>
     </row>
@@ -2570,10 +2456,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F69" t="n">
+        <v>45</v>
       </c>
       <c r="G69" t="inlineStr"/>
     </row>
@@ -2601,10 +2485,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F70" t="n">
+        <v>33</v>
       </c>
       <c r="G70" t="inlineStr"/>
     </row>
@@ -2632,10 +2514,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F71" t="n">
+        <v>68</v>
       </c>
       <c r="G71" t="inlineStr"/>
     </row>
@@ -2663,10 +2543,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F72" t="n">
+        <v>39</v>
       </c>
       <c r="G72" t="inlineStr"/>
     </row>
@@ -2694,10 +2572,8 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="F73" t="n">
+        <v>42</v>
       </c>
       <c r="G73" t="inlineStr"/>
     </row>

</xml_diff>